<commit_message>
Lab 2 done. Seems like don't work if there are both >= and <= as input
</commit_message>
<xml_diff>
--- a/Lab2/simplexmethod.xlsx
+++ b/Lab2/simplexmethod.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18345" windowHeight="7980"/>
+    <workbookView windowWidth="27945" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,20 +50,7 @@
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -151,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -324,7 +311,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,12 +326,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -435,12 +416,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -526,12 +501,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,7 +670,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -725,16 +694,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -743,165 +712,150 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1486,8 +1440,8 @@
   <sheetPr/>
   <dimension ref="A5:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1515,22 +1469,22 @@
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M6" s="1" t="s">
@@ -1557,34 +1511,34 @@
         <f>B8+B9</f>
         <v>7</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>1</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>-1</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>-1</v>
       </c>
-      <c r="J7" s="19">
-        <v>0</v>
-      </c>
-      <c r="K7" s="19">
-        <v>0</v>
-      </c>
-      <c r="L7" s="19">
-        <v>0</v>
-      </c>
-      <c r="M7" s="20">
-        <v>0</v>
-      </c>
-      <c r="N7" s="21"/>
+      <c r="J7" s="14">
+        <v>0</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
+      <c r="M7" s="15">
+        <v>0</v>
+      </c>
+      <c r="N7" s="16"/>
       <c r="P7" t="s">
         <v>5</v>
       </c>
@@ -1605,34 +1559,34 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>2</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
         <v>2</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>11</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="14">
         <v>1</v>
       </c>
-      <c r="K8" s="19">
-        <v>0</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0</v>
-      </c>
-      <c r="M8" s="20">
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
+      <c r="M8" s="15">
         <v>38</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="16">
         <f>M8/H8</f>
         <v>19</v>
       </c>
@@ -1647,34 +1601,34 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>3</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
         <v>1</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>1</v>
       </c>
-      <c r="J9" s="19">
-        <v>0</v>
-      </c>
-      <c r="K9" s="19">
+      <c r="J9" s="14">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14">
         <v>1</v>
       </c>
-      <c r="L9" s="19">
-        <v>0</v>
-      </c>
-      <c r="M9" s="20">
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9" s="15">
         <v>7</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="16">
         <f>M9/H9</f>
         <v>7</v>
       </c>
@@ -1696,34 +1650,34 @@
       <c r="C10">
         <v>38</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>4</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="7">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7">
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
         <v>4</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>-5</v>
       </c>
-      <c r="J10" s="22">
-        <v>0</v>
-      </c>
-      <c r="K10" s="22">
-        <v>0</v>
-      </c>
-      <c r="L10" s="22">
+      <c r="J10" s="17">
+        <v>0</v>
+      </c>
+      <c r="K10" s="17">
+        <v>0</v>
+      </c>
+      <c r="L10" s="17">
         <v>1</v>
       </c>
-      <c r="M10" s="20">
+      <c r="M10" s="15">
         <v>5</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="16">
         <f>M10/H10</f>
         <v>1.25</v>
       </c>
@@ -1754,7 +1708,7 @@
       </c>
       <c r="B12">
         <f>4*B8-5*B9</f>
-        <v>5</v>
+        <v>4.99999999999996</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1767,31 +1721,31 @@
       <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P13" t="s">
@@ -1805,41 +1759,41 @@
       </c>
     </row>
     <row r="14" spans="5:18">
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="13">
-        <f>G7-G17*$H$7</f>
+      <c r="G14" s="10">
+        <f t="shared" ref="G14:M14" si="0">G7-G17*$H$7</f>
         <v>1</v>
       </c>
-      <c r="H14" s="13">
-        <f>H7-H17*$H$7</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="7">
-        <f>I7-I17*$H$7</f>
+      <c r="H14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="0"/>
         <v>-2.25</v>
       </c>
-      <c r="J14" s="13">
-        <f>J7-J17*$H$7</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="13">
-        <f>K7-K17*$H$7</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="13">
-        <f>L7-L17*$H$7</f>
+      <c r="J14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="10">
         <f>M7-M17*$H$7</f>
         <v>1.25</v>
       </c>
-      <c r="N14" s="23"/>
+      <c r="N14" s="18"/>
       <c r="P14" t="s">
         <v>6</v>
       </c>
@@ -1851,81 +1805,81 @@
       </c>
     </row>
     <row r="15" spans="5:14">
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>2</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="13">
-        <f>G8-G17*$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="13">
-        <f>H8-H17*$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="7">
-        <f>I8-I17*$H$8</f>
+      <c r="G15" s="10">
+        <f t="shared" ref="G15:M15" si="1">G8-G17*$H$8</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="J15" s="13">
-        <f>J8-J17*$H$8</f>
+      <c r="J15" s="10">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K15" s="13">
-        <f>K8-K17*$H$8</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="13">
-        <f>L8-L17*$H$8</f>
+      <c r="K15" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
-      <c r="M15" s="13">
-        <f>M8-M17*$H$8</f>
+      <c r="M15" s="10">
+        <f t="shared" si="1"/>
         <v>35.5</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="18">
         <f>M15/I15</f>
         <v>2.62962962962963</v>
       </c>
     </row>
     <row r="16" spans="5:17">
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>3</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="7">
-        <f>G9-G17*$H$9</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="7">
-        <f>H9-H17*$H$9</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="7">
-        <f>I9-I17*$H$9</f>
+      <c r="G16" s="6">
+        <f t="shared" ref="G16:M16" si="2">G9-G17*$H$9</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="2"/>
         <v>2.25</v>
       </c>
-      <c r="J16" s="7">
-        <f>J9-J17*$H$9</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="7">
-        <f>K9-K17*$H$9</f>
+      <c r="J16" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L16" s="7">
-        <f>L9-L17*$H$9</f>
+      <c r="L16" s="6">
+        <f t="shared" si="2"/>
         <v>-0.25</v>
       </c>
-      <c r="M16" s="7">
-        <f>M9-M17*$H$9</f>
+      <c r="M16" s="6">
+        <f t="shared" si="2"/>
         <v>5.75</v>
       </c>
-      <c r="N16" s="24">
+      <c r="N16" s="19">
         <f>M16/I16</f>
         <v>2.55555555555556</v>
       </c>
@@ -1937,41 +1891,41 @@
       </c>
     </row>
     <row r="17" spans="5:17">
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>4</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="13">
-        <f>G10/$R$7</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="13">
+      <c r="G17" s="10">
+        <f t="shared" ref="G17:M17" si="3">G10/$R$7</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
         <f>H10/$R$7</f>
         <v>1</v>
       </c>
-      <c r="I17" s="7">
-        <f>I10/$R$7</f>
+      <c r="I17" s="6">
+        <f t="shared" si="3"/>
         <v>-1.25</v>
       </c>
-      <c r="J17" s="13">
-        <f>J10/$R$7</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="13">
-        <f>K10/$R$7</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="13">
-        <f>L10/$R$7</f>
+      <c r="J17" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="M17" s="13">
-        <f>M10/$R$7</f>
+      <c r="M17" s="10">
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="18">
         <f>M17/I17</f>
         <v>-1</v>
       </c>
@@ -1993,31 +1947,31 @@
       <c r="E20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="16" t="s">
+      <c r="J20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="16" t="s">
+      <c r="K20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L20" s="16" t="s">
+      <c r="L20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="M20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="N20" s="15" t="s">
+      <c r="N20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="P20" t="s">
@@ -2031,115 +1985,115 @@
       </c>
     </row>
     <row r="21" spans="5:14">
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="18">
-        <f>G14-G23*$I$14</f>
+      <c r="G21" s="13">
+        <f t="shared" ref="G21:M21" si="4">G14-G23*$I$14</f>
         <v>1</v>
       </c>
-      <c r="H21" s="18">
-        <f>H14-H23*$I$14</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="18">
-        <f>I14-I23*$I$14</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="18">
-        <f>J14-J23*$I$14</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="18">
-        <f>K14-K23*$I$14</f>
+      <c r="H21" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L21" s="18">
-        <f>L14-L23*$I$14</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="18">
-        <f>M14-M23*$I$14</f>
+      <c r="L21" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="13">
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="N21" s="25"/>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="5:14">
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>2</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="18">
-        <f>G15-G23*$I$15</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="18">
-        <f>H15-H23*$I$15</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="18">
-        <f>I15-I23*$I$15</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="18">
-        <f>J15-J23*$I$15</f>
+      <c r="G22" s="13">
+        <f t="shared" ref="G22:M22" si="5">G15-G23*$I$15</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="13">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="K22" s="18">
-        <f>K15-K23*$I$15</f>
+      <c r="K22" s="13">
+        <f t="shared" si="5"/>
         <v>-6</v>
       </c>
-      <c r="L22" s="18">
-        <f>L15-L23*$I$15</f>
+      <c r="L22" s="13">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="M22" s="18">
-        <f>M15-M23*$I$15</f>
+      <c r="M22" s="13">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="N22" s="25"/>
+      <c r="N22" s="20"/>
     </row>
     <row r="23" spans="5:17">
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>3</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="18">
-        <f>G16/$R$14</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="18">
-        <f>H16/$R$14</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="18">
-        <f>I16/$R$14</f>
+      <c r="G23" s="13">
+        <f t="shared" ref="G23:M23" si="6">G16/$R$14</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="13">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="J23" s="18">
-        <f>J16/$R$14</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="18">
-        <f>K16/$R$14</f>
+      <c r="J23" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="13">
+        <f t="shared" si="6"/>
         <v>0.444444444444444</v>
       </c>
-      <c r="L23" s="18">
-        <f>L16/$R$14</f>
+      <c r="L23" s="13">
+        <f t="shared" si="6"/>
         <v>-0.111111111111111</v>
       </c>
-      <c r="M23" s="18">
-        <f>M16/$R$14</f>
+      <c r="M23" s="13">
+        <f t="shared" si="6"/>
         <v>2.55555555555556</v>
       </c>
-      <c r="N23" s="25"/>
+      <c r="N23" s="20"/>
       <c r="P23" t="s">
         <v>15</v>
       </c>
@@ -2148,41 +2102,41 @@
       </c>
     </row>
     <row r="24" spans="5:16">
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>4</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="18">
-        <f>G17-G23*$I$17</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="18">
-        <f>H17-H23*$I$17</f>
+      <c r="G24" s="13">
+        <f t="shared" ref="G24:M24" si="7">G17-G23*$I$17</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="I24" s="18">
-        <f>I17-I23*$I$17</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="18">
-        <f>J17-J23*$I$17</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="18">
-        <f>K17-K23*$I$17</f>
+      <c r="I24" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="13">
+        <f t="shared" si="7"/>
         <v>0.555555555555556</v>
       </c>
-      <c r="L24" s="18">
-        <f>L17-L23*$I$17</f>
+      <c r="L24" s="13">
+        <f t="shared" si="7"/>
         <v>0.111111111111111</v>
       </c>
-      <c r="M24" s="18">
-        <f>M17-M23*$I$17</f>
+      <c r="M24" s="13">
+        <f t="shared" si="7"/>
         <v>4.44444444444444</v>
       </c>
-      <c r="N24" s="25"/>
+      <c r="N24" s="20"/>
       <c r="P24" t="str">
         <f>IF(MIN(H21:L21)&lt;0,MIN(H21:L21),"Optimal")</f>
         <v>Optimal</v>

</xml_diff>